<commit_message>
Auto-committed on 2022/02/14 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/測試FT/L5/L5060/FT_L5060.xlsx
+++ b/Program/Other/Sharepoint上傳用/測試FT/L5/L5060/FT_L5060.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\測試FT\L5\L5060\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15556B9-3F9E-407D-8AC6-3553BF74CB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2807A5-85CD-4F91-A62F-3F84363ECB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,9 +441,6 @@
     <t>L5</t>
   </si>
   <si>
-    <t>製作依據之需求規格書與版本：PJ201800012_URS_5管理性作業_V1.65.docx</t>
-  </si>
-  <si>
     <t>1.當[查詢身分別]等於1~3時可不輸入,預設值為0
 2.若有輸入則限輸入代碼,檢核條件：依選單/V(H)
 以下欄位[逾期期數]、[逾期天數]依[逾期期數/天數]欄位值分別顯示</t>
@@ -457,6 +454,9 @@
   <si>
     <t>1.預設值為00全部,若有輸入則限輸入空白或代碼，不為空白時，檢核條件：依選單/V(H)</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>製作依據之需求規格書與版本：PJ201800012_URS_5管理性作業_V1.64.DOCX</t>
   </si>
 </sst>
 </file>
@@ -981,7 +981,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.2"/>
@@ -1092,7 +1092,7 @@
         <v>15</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>21</v>
@@ -1136,7 +1136,7 @@
         <v>15</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -1182,7 +1182,7 @@
         <v>110</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1228,7 +1228,7 @@
         <v>110</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1277,7 +1277,7 @@
         <v>110</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1372,7 +1372,7 @@
         <v>110</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1418,7 +1418,7 @@
         <v>110</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1467,7 +1467,7 @@
         <v>110</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1513,7 +1513,7 @@
         <v>110</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1562,7 +1562,7 @@
         <v>110</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1609,7 +1609,7 @@
         <v>110</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1658,7 +1658,7 @@
         <v>110</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1704,7 +1704,7 @@
         <v>110</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1750,7 +1750,7 @@
         <v>110</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -1778,7 +1778,7 @@
         <v>59</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>12</v>
@@ -1796,7 +1796,7 @@
         <v>110</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1842,7 +1842,7 @@
         <v>110</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1888,7 +1888,7 @@
         <v>110</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1916,7 +1916,7 @@
         <v>64</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>12</v>
@@ -1934,7 +1934,7 @@
         <v>110</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1962,7 +1962,7 @@
         <v>65</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>12</v>
@@ -1980,7 +1980,7 @@
         <v>110</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -2026,7 +2026,7 @@
         <v>110</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -2075,7 +2075,7 @@
         <v>110</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -2124,7 +2124,7 @@
         <v>110</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -2173,7 +2173,7 @@
         <v>110</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -2222,7 +2222,7 @@
         <v>110</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
@@ -2271,7 +2271,7 @@
         <v>110</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -2320,7 +2320,7 @@
         <v>110</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -2369,7 +2369,7 @@
         <v>110</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -2418,7 +2418,7 @@
         <v>110</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -2467,7 +2467,7 @@
         <v>110</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
@@ -2516,7 +2516,7 @@
         <v>110</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
@@ -2565,7 +2565,7 @@
         <v>110</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -2614,7 +2614,7 @@
         <v>110</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -2663,7 +2663,7 @@
         <v>110</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
@@ -2712,7 +2712,7 @@
         <v>110</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
@@ -2761,7 +2761,7 @@
         <v>110</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
@@ -2810,7 +2810,7 @@
         <v>110</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
@@ -2859,7 +2859,7 @@
         <v>110</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
@@ -2908,7 +2908,7 @@
         <v>110</v>
       </c>
       <c r="M40" s="11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N40" s="11"/>
       <c r="O40" s="11"/>

</xml_diff>